<commit_message>
Mundança no layout do simulador
</commit_message>
<xml_diff>
--- a/projeto-site/public/pages/Simulador/teste de mesa-simulador.xlsx
+++ b/projeto-site/public/pages/Simulador/teste de mesa-simulador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Faculdade\PESQUISA E INOVAÇÃO\Projeto-Sprint3\TechCare\TechCare-Sprint-3\projeto-site\public\pages\Simulador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED158F2-8452-4AE1-B6AA-0DEFA35EBFCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECF94EC-621B-453A-80A9-2EFC49AB9638}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7F32D02C-A626-4595-AEF2-EB22B615A870}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7F32D02C-A626-4595-AEF2-EB22B615A870}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -189,19 +189,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -521,32 +521,32 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="15.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="2"/>
-    <col min="5" max="7" width="17.08984375" style="2" customWidth="1"/>
+    <col min="1" max="2" width="15.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="2"/>
+    <col min="5" max="7" width="17.109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="18" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" ht="18">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="4"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
@@ -575,95 +575,95 @@
       <c r="A3" s="1">
         <v>200</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1">
         <v>200</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>300</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1">
         <v>300</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>500</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>500</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>100</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1">
         <v>100</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>50</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="1">
         <v>50</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="1"/>
     </row>
     <row r="12" spans="1:8">

</xml_diff>